<commit_message>
add sample data to excel
</commit_message>
<xml_diff>
--- a/Post/Index/data/Distribusi Data Kelembapan.xlsx
+++ b/Post/Index/data/Distribusi Data Kelembapan.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>78207</v>
+        <v>78206</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>95.28082038692187</v>
+        <v>95.28203104621129</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8.557211915909097</v>
+        <v>8.550566236222211</v>
       </c>
     </row>
     <row r="5">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6</v>
+        <v>36.09</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
revisi 09 April 2025
</commit_message>
<xml_diff>
--- a/Post/Index/data/Distribusi Data Kelembapan.xlsx
+++ b/Post/Index/data/Distribusi Data Kelembapan.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>78206</v>
+        <v>31629</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>95.28203104621129</v>
+        <v>92.06928040722123</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8.550566236222211</v>
+        <v>10.1529448215195</v>
       </c>
     </row>
     <row r="5">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>36.09</v>
+        <v>47.44</v>
       </c>
     </row>
     <row r="6">
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>95.16</v>
+        <v>85.31</v>
       </c>
     </row>
     <row r="7">
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>100</v>
+        <v>97.39</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
fixed revisi persiapan seminar hasil
</commit_message>
<xml_diff>
--- a/Post/Index/data/Distribusi Data Kelembapan.xlsx
+++ b/Post/Index/data/Distribusi Data Kelembapan.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>47733</v>
+        <v>47548</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>93.20748748245448</v>
+        <v>92.43986077227223</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10.16899924485133</v>
+        <v>10.68069421272411</v>
       </c>
     </row>
     <row r="5">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>63.3</v>
+        <v>47.44</v>
       </c>
     </row>
     <row r="6">
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>85.59</v>
+        <v>89.0675</v>
       </c>
     </row>
     <row r="7">
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>100</v>
+        <v>97.91</v>
       </c>
     </row>
     <row r="8">

</xml_diff>